<commit_message>
application for financialfacility commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_FMS_Batch/TestData/FMSTestData.xlsx
+++ b/AzentioAutomationFramework_FMS_Batch/TestData/FMSTestData.xlsx
@@ -4,33 +4,36 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9228" tabRatio="806" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="806" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="AllFeaturesTestExecutionInfo" sheetId="1" r:id="rId1"/>
     <sheet name="AllFeaturesTestDataInstructions" sheetId="2" r:id="rId2"/>
     <sheet name="CSMParam_Login" sheetId="3" r:id="rId3"/>
     <sheet name="CSM_Login" sheetId="4" r:id="rId4"/>
-    <sheet name="FMS_Login" sheetId="5" r:id="rId5"/>
-    <sheet name="FMSParam_login" sheetId="6" r:id="rId6"/>
+    <sheet name="FMS_Login" sheetId="22" r:id="rId5"/>
+    <sheet name="FMSParam_login" sheetId="23" r:id="rId6"/>
     <sheet name="IISParam_Login" sheetId="7" r:id="rId7"/>
     <sheet name="SadsLogin" sheetId="8" r:id="rId8"/>
     <sheet name="TestExecution" sheetId="9" r:id="rId9"/>
-    <sheet name="IIS_Param_TestData" sheetId="11" r:id="rId10"/>
-    <sheet name="FMS_WIFAK_ApplicationTestData" sheetId="12" r:id="rId11"/>
-    <sheet name="Request_For_FinancingTestData" sheetId="15" r:id="rId12"/>
-    <sheet name="FMS_Collateral_Management" sheetId="13" r:id="rId13"/>
-    <sheet name="Draw_Down_Request" sheetId="14" r:id="rId14"/>
-    <sheet name="FacilitiesManagementTestData" sheetId="16" r:id="rId15"/>
-    <sheet name="ApplicationFinancialFacility" sheetId="17" r:id="rId16"/>
-    <sheet name="FMSParameterTestData" sheetId="18" r:id="rId17"/>
+    <sheet name="WIFAK_Application_609" sheetId="25" r:id="rId10"/>
+    <sheet name="IIS_Param_TestData" sheetId="11" r:id="rId11"/>
+    <sheet name="WIFAK_Application_Testdata" sheetId="19" r:id="rId12"/>
+    <sheet name="FMS_WIFAK_Application_610" sheetId="24" r:id="rId13"/>
+    <sheet name="FMS_WIFAK_ApplicationTestData" sheetId="12" r:id="rId14"/>
+    <sheet name="Request_For_FinancingTestData" sheetId="15" r:id="rId15"/>
+    <sheet name="FMS_Collateral_Management" sheetId="13" r:id="rId16"/>
+    <sheet name="Draw_Down_Request" sheetId="14" r:id="rId17"/>
+    <sheet name="FacilitiesManagementTestData" sheetId="16" r:id="rId18"/>
+    <sheet name="ApplicationFinancialFacility" sheetId="17" r:id="rId19"/>
+    <sheet name="FMSParameterTestData" sheetId="18" r:id="rId20"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="340">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -813,10 +816,247 @@
     <t>Month(s)</t>
   </si>
   <si>
-    <t>4499</t>
-  </si>
-  <si>
     <t>4504</t>
+  </si>
+  <si>
+    <t>Total Value</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Cy</t>
+  </si>
+  <si>
+    <t>UnitCost</t>
+  </si>
+  <si>
+    <t>Down Payment High</t>
+  </si>
+  <si>
+    <t>Down Payment Less</t>
+  </si>
+  <si>
+    <t>Approve2 Decision</t>
+  </si>
+  <si>
+    <t>Approve3 Decision</t>
+  </si>
+  <si>
+    <t>Product Class 1</t>
+  </si>
+  <si>
+    <t>Product Class 2</t>
+  </si>
+  <si>
+    <t>Facility Value</t>
+  </si>
+  <si>
+    <t>Floating Rate Periodicity</t>
+  </si>
+  <si>
+    <t>Floating Rate Periodicity Type</t>
+  </si>
+  <si>
+    <t>ApplicationFor</t>
+  </si>
+  <si>
+    <t>Existing Facility Ref</t>
+  </si>
+  <si>
+    <t>Total value on additional Details</t>
+  </si>
+  <si>
+    <t>Change Down Payment</t>
+  </si>
+  <si>
+    <t>AT_AFF_017</t>
+  </si>
+  <si>
+    <t>25/05/2023</t>
+  </si>
+  <si>
+    <t>AT_AFF_012</t>
+  </si>
+  <si>
+    <t>AT_AFF_022</t>
+  </si>
+  <si>
+    <t>AT_AFF_057</t>
+  </si>
+  <si>
+    <t>AT_FM_017</t>
+  </si>
+  <si>
+    <t>AT_AFF_007</t>
+  </si>
+  <si>
+    <t>AT_RF_113</t>
+  </si>
+  <si>
+    <t>AT_RF_055</t>
+  </si>
+  <si>
+    <t>CHRISAG</t>
+  </si>
+  <si>
+    <t>FMS_User3</t>
+  </si>
+  <si>
+    <t>AJITH</t>
+  </si>
+  <si>
+    <t>FMS_User4</t>
+  </si>
+  <si>
+    <t>FMS_User5</t>
+  </si>
+  <si>
+    <t>JAY</t>
+  </si>
+  <si>
+    <t>FMS_User6</t>
+  </si>
+  <si>
+    <t>SNEHA</t>
+  </si>
+  <si>
+    <t>FMS_User7</t>
+  </si>
+  <si>
+    <t>KOUSALYA</t>
+  </si>
+  <si>
+    <t>FMS_User8</t>
+  </si>
+  <si>
+    <t>ARUL</t>
+  </si>
+  <si>
+    <t>FMS_User9</t>
+  </si>
+  <si>
+    <t>PRIYANKA</t>
+  </si>
+  <si>
+    <t>FMS_User10</t>
+  </si>
+  <si>
+    <t>RAJAT</t>
+  </si>
+  <si>
+    <t>FMS_User11</t>
+  </si>
+  <si>
+    <t>VIJAYK</t>
+  </si>
+  <si>
+    <t>FMS_User12</t>
+  </si>
+  <si>
+    <t>GOWTHAM</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser3</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser4</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser5</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser6</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser7</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser8</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser9</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser10</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser11</t>
+  </si>
+  <si>
+    <t>FMS_ParamUser12</t>
+  </si>
+  <si>
+    <t>Application Ref No in Facilities Management</t>
+  </si>
+  <si>
+    <t>Maturity Date facility management</t>
+  </si>
+  <si>
+    <t>Down Payment</t>
+  </si>
+  <si>
+    <t>Expected Payment Date</t>
+  </si>
+  <si>
+    <t>Total Down Payment</t>
+  </si>
+  <si>
+    <t>DS01_870478</t>
+  </si>
+  <si>
+    <t>14/06/2023</t>
+  </si>
+  <si>
+    <t>DS01_1038991</t>
+  </si>
+  <si>
+    <t>DS01_665893</t>
+  </si>
+  <si>
+    <t>DS01_592970</t>
+  </si>
+  <si>
+    <t>02/10/2022</t>
+  </si>
+  <si>
+    <t>DS01_592279</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Revolving/One-Off</t>
+  </si>
+  <si>
+    <t>MarketedBY</t>
+  </si>
+  <si>
+    <t>DS01_326257</t>
+  </si>
+  <si>
+    <t>DS01_402669</t>
+  </si>
+  <si>
+    <t>Revolving</t>
+  </si>
+  <si>
+    <t>DS01_834958</t>
+  </si>
+  <si>
+    <t>DS01_127780</t>
+  </si>
+  <si>
+    <t>DS01_402668</t>
   </si>
 </sst>
 </file>
@@ -827,7 +1067,7 @@
     <numFmt numFmtId="164" formatCode="dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -903,8 +1143,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -983,8 +1229,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1098,8 +1356,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1113,8 +1406,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1316,9 +1610,58 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="ConditionalStyle_5f_1" xfId="7"/>
+    <cellStyle name="Excel Built-in Normal" xfId="9"/>
     <cellStyle name="Excel_20_Built-in_20_Normal" xfId="8"/>
     <cellStyle name="Excel_5f_20_5f_Built-in_5f_20_5f_Normal" xfId="5"/>
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="6"/>
@@ -1655,7 +1998,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1670,17 +2013,17 @@
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="32.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="13.33203125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="3" width="12.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="3" width="15.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="15.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="3" width="13.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="16.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="34.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="3" width="15.0" collapsed="true"/>
-    <col min="10" max="16384" style="3" width="32.33203125" collapsed="true"/>
+    <col min="1" max="1" width="13.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="12.7109375" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="32.28515625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3699,24 +4042,598 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AB14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="9" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="26.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" customWidth="1"/>
+    <col min="21" max="21" width="21.5703125" customWidth="1"/>
+    <col min="22" max="22" width="19.7109375" customWidth="1"/>
+    <col min="23" max="23" width="8.140625" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" customWidth="1"/>
+    <col min="27" max="27" width="19.28515625" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="124" customFormat="1" ht="30">
+      <c r="A1" s="121" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="121" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="122" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" s="122" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="122" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="122" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="122" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="122" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="122" t="s">
+        <v>332</v>
+      </c>
+      <c r="K1" s="122" t="s">
+        <v>333</v>
+      </c>
+      <c r="L1" s="122" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="123" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="122" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" s="122" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="122" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="122" t="s">
+        <v>113</v>
+      </c>
+      <c r="R1" s="122" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="122" t="s">
+        <v>114</v>
+      </c>
+      <c r="T1" s="122" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" s="122" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" s="122" t="s">
+        <v>103</v>
+      </c>
+      <c r="W1" s="122" t="s">
+        <v>104</v>
+      </c>
+      <c r="X1" s="122" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" s="122" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z1" s="122" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA1" s="122" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="121" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="35">
+        <v>326257</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37">
+        <v>727</v>
+      </c>
+      <c r="G2" s="37">
+        <v>369</v>
+      </c>
+      <c r="H2" s="37">
+        <v>320</v>
+      </c>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="41"/>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" s="35">
+        <v>402669</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="41"/>
+      <c r="F3" s="37">
+        <v>727</v>
+      </c>
+      <c r="G3" s="41">
+        <v>369</v>
+      </c>
+      <c r="H3" s="41">
+        <v>840</v>
+      </c>
+      <c r="I3" s="41">
+        <v>2</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="K3" s="38"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" s="35">
+        <v>834958</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>337</v>
+      </c>
+      <c r="C4" s="41"/>
+      <c r="D4" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37">
+        <v>727</v>
+      </c>
+      <c r="G4" s="41">
+        <v>369</v>
+      </c>
+      <c r="H4" s="37">
+        <v>320</v>
+      </c>
+      <c r="I4" s="41">
+        <v>2</v>
+      </c>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37">
+        <v>180456</v>
+      </c>
+      <c r="L4" s="37"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="41"/>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" s="35">
+        <v>127780</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="C5" s="37">
+        <v>221</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="38"/>
+      <c r="Y5" s="38"/>
+      <c r="Z5" s="36"/>
+      <c r="AA5" s="36"/>
+      <c r="AB5" s="41"/>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" s="35">
+        <v>402668</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>339</v>
+      </c>
+      <c r="C6" s="37">
+        <v>221</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="36"/>
+      <c r="AB6" s="41"/>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+    </row>
+    <row r="8" spans="1:28">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="37"/>
+    </row>
+    <row r="9" spans="1:28">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
+    </row>
+    <row r="10" spans="1:28">
+      <c r="A10" s="42"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="36"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="A11" s="42"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+    </row>
+    <row r="12" spans="1:28">
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="36"/>
+      <c r="AA12" s="41"/>
+      <c r="AB12" s="41"/>
+    </row>
+    <row r="13" spans="1:28">
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="36"/>
+      <c r="AA13" s="41"/>
+      <c r="AB13" s="41"/>
+    </row>
+    <row r="14" spans="1:28">
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="38"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="36"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="7" max="13" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="13" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4">
+    <row r="1" spans="1:13" ht="15">
       <c r="A1" s="17" t="s">
         <v>34</v>
       </c>
@@ -3808,48 +4725,1563 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AH9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" customWidth="1"/>
+    <col min="23" max="23" width="17.5703125" customWidth="1"/>
+    <col min="24" max="24" width="16.28515625" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" customWidth="1"/>
+    <col min="26" max="26" width="15.28515625" customWidth="1"/>
+    <col min="29" max="29" width="23.42578125" customWidth="1"/>
+    <col min="30" max="30" width="28.28515625" customWidth="1"/>
+    <col min="31" max="31" width="15" customWidth="1"/>
+    <col min="32" max="32" width="19" customWidth="1"/>
+    <col min="33" max="33" width="34.42578125" customWidth="1"/>
+    <col min="34" max="34" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" ht="15">
+      <c r="A1" s="93" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="100" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="100" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="100" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="100" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="100" t="s">
+        <v>260</v>
+      </c>
+      <c r="I1" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="101" t="s">
+        <v>261</v>
+      </c>
+      <c r="L1" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="102" t="s">
+        <v>262</v>
+      </c>
+      <c r="N1" s="102" t="s">
+        <v>263</v>
+      </c>
+      <c r="O1" s="101" t="s">
+        <v>264</v>
+      </c>
+      <c r="P1" s="101" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q1" s="101" t="s">
+        <v>266</v>
+      </c>
+      <c r="R1" s="101" t="s">
+        <v>267</v>
+      </c>
+      <c r="S1" s="101" t="s">
+        <v>268</v>
+      </c>
+      <c r="T1" s="101" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" s="101" t="s">
+        <v>76</v>
+      </c>
+      <c r="V1" s="101" t="s">
+        <v>202</v>
+      </c>
+      <c r="W1" s="101" t="s">
+        <v>269</v>
+      </c>
+      <c r="X1" s="101" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y1" s="101" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z1" s="101" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA1" s="101" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB1" s="101" t="s">
+        <v>255</v>
+      </c>
+      <c r="AC1" s="101" t="s">
+        <v>274</v>
+      </c>
+      <c r="AD1" s="101" t="s">
+        <v>275</v>
+      </c>
+      <c r="AE1" s="101" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF1" s="103" t="s">
+        <v>277</v>
+      </c>
+      <c r="AG1" s="101" t="s">
+        <v>278</v>
+      </c>
+      <c r="AH1" s="101" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="15.75">
+      <c r="A2" s="104">
+        <v>917005</v>
+      </c>
+      <c r="B2" s="105" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="106">
+        <v>727</v>
+      </c>
+      <c r="E2" s="106">
+        <v>369</v>
+      </c>
+      <c r="F2" s="106">
+        <v>320</v>
+      </c>
+      <c r="G2" s="106">
+        <v>2</v>
+      </c>
+      <c r="H2" s="106">
+        <v>10000</v>
+      </c>
+      <c r="I2" s="107" t="s">
+        <v>281</v>
+      </c>
+      <c r="J2" s="106">
+        <v>160</v>
+      </c>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="108"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="108"/>
+      <c r="T2" s="108"/>
+      <c r="U2" s="108"/>
+      <c r="V2" s="109"/>
+      <c r="W2" s="109"/>
+      <c r="X2" s="109"/>
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="108"/>
+      <c r="AA2" s="108"/>
+      <c r="AB2" s="108"/>
+      <c r="AC2" s="108"/>
+      <c r="AD2" s="108"/>
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="108"/>
+      <c r="AG2" s="108"/>
+      <c r="AH2" s="108"/>
+    </row>
+    <row r="3" spans="1:34">
+      <c r="A3" s="47">
+        <v>949677</v>
+      </c>
+      <c r="B3" s="92" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="106">
+        <v>727</v>
+      </c>
+      <c r="E3" s="106">
+        <v>369</v>
+      </c>
+      <c r="F3" s="106">
+        <v>320</v>
+      </c>
+      <c r="G3" s="106">
+        <v>2</v>
+      </c>
+      <c r="H3" s="106">
+        <v>10000</v>
+      </c>
+      <c r="I3" s="107" t="s">
+        <v>281</v>
+      </c>
+      <c r="J3" s="106">
+        <v>160</v>
+      </c>
+      <c r="K3" s="106">
+        <v>1</v>
+      </c>
+      <c r="L3" s="106">
+        <v>1234</v>
+      </c>
+      <c r="M3" s="106">
+        <v>1</v>
+      </c>
+      <c r="N3" s="106">
+        <v>11</v>
+      </c>
+      <c r="O3" s="106">
+        <v>11</v>
+      </c>
+      <c r="P3" s="106">
+        <v>999</v>
+      </c>
+      <c r="Q3" s="106">
+        <v>11</v>
+      </c>
+      <c r="R3" s="108"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="108"/>
+      <c r="Z3" s="108"/>
+      <c r="AA3" s="108"/>
+      <c r="AB3" s="108"/>
+      <c r="AC3" s="108"/>
+      <c r="AD3" s="108"/>
+      <c r="AE3" s="108"/>
+      <c r="AF3" s="108"/>
+      <c r="AG3" s="108"/>
+      <c r="AH3" s="108"/>
+    </row>
+    <row r="4" spans="1:34">
+      <c r="A4" s="47">
+        <v>817662</v>
+      </c>
+      <c r="B4" s="92" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="106">
+        <v>727</v>
+      </c>
+      <c r="E4" s="106">
+        <v>369</v>
+      </c>
+      <c r="F4" s="106">
+        <v>320</v>
+      </c>
+      <c r="G4" s="106">
+        <v>2</v>
+      </c>
+      <c r="H4" s="106">
+        <v>10000</v>
+      </c>
+      <c r="I4" s="107" t="s">
+        <v>281</v>
+      </c>
+      <c r="J4" s="106">
+        <v>160</v>
+      </c>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="108"/>
+      <c r="Q4" s="108"/>
+      <c r="R4" s="108"/>
+      <c r="S4" s="108"/>
+      <c r="T4" s="108"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109"/>
+      <c r="X4" s="109"/>
+      <c r="Y4" s="108"/>
+      <c r="Z4" s="108"/>
+      <c r="AA4" s="108"/>
+      <c r="AB4" s="108"/>
+      <c r="AC4" s="108"/>
+      <c r="AD4" s="108"/>
+      <c r="AE4" s="108"/>
+      <c r="AF4" s="108"/>
+      <c r="AG4" s="108"/>
+      <c r="AH4" s="108"/>
+    </row>
+    <row r="5" spans="1:34">
+      <c r="A5" s="47">
+        <v>299886</v>
+      </c>
+      <c r="B5" s="92" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="106">
+        <v>727</v>
+      </c>
+      <c r="E5" s="106">
+        <v>369</v>
+      </c>
+      <c r="F5" s="106">
+        <v>320</v>
+      </c>
+      <c r="G5" s="106">
+        <v>2</v>
+      </c>
+      <c r="H5" s="106">
+        <v>10000</v>
+      </c>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="108">
+        <v>100</v>
+      </c>
+      <c r="S5" s="108">
+        <v>10000</v>
+      </c>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="108"/>
+      <c r="Z5" s="108"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="108"/>
+      <c r="AC5" s="108"/>
+      <c r="AD5" s="108"/>
+      <c r="AE5" s="108"/>
+      <c r="AF5" s="108"/>
+      <c r="AG5" s="108"/>
+      <c r="AH5" s="108"/>
+    </row>
+    <row r="6" spans="1:34" ht="15">
+      <c r="A6" s="47">
+        <v>539219</v>
+      </c>
+      <c r="B6" s="110" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="106">
+        <v>727</v>
+      </c>
+      <c r="E6" s="106">
+        <v>369</v>
+      </c>
+      <c r="F6" s="106">
+        <v>320</v>
+      </c>
+      <c r="G6" s="106">
+        <v>2</v>
+      </c>
+      <c r="H6" s="106">
+        <v>10000</v>
+      </c>
+      <c r="I6" s="107" t="s">
+        <v>281</v>
+      </c>
+      <c r="J6" s="106">
+        <v>160</v>
+      </c>
+      <c r="K6" s="108"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="108"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="108"/>
+      <c r="Q6" s="108"/>
+      <c r="R6" s="108"/>
+      <c r="S6" s="108"/>
+      <c r="T6" s="108">
+        <v>1</v>
+      </c>
+      <c r="U6" s="108">
+        <v>1</v>
+      </c>
+      <c r="V6" s="109" t="s">
+        <v>201</v>
+      </c>
+      <c r="W6" s="109" t="s">
+        <v>201</v>
+      </c>
+      <c r="X6" s="109" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y6" s="108"/>
+      <c r="Z6" s="108"/>
+      <c r="AA6" s="108"/>
+      <c r="AB6" s="108"/>
+      <c r="AC6" s="108"/>
+      <c r="AD6" s="108"/>
+      <c r="AE6" s="108"/>
+      <c r="AF6" s="108"/>
+      <c r="AG6" s="108"/>
+      <c r="AH6" s="108"/>
+    </row>
+    <row r="7" spans="1:34" ht="15">
+      <c r="A7" s="111">
+        <v>929306</v>
+      </c>
+      <c r="B7" s="92" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="106">
+        <v>727</v>
+      </c>
+      <c r="E7" s="106">
+        <v>369</v>
+      </c>
+      <c r="F7" s="106">
+        <v>320</v>
+      </c>
+      <c r="G7" s="106">
+        <v>2</v>
+      </c>
+      <c r="H7" s="106">
+        <v>10000</v>
+      </c>
+      <c r="I7" s="107" t="s">
+        <v>281</v>
+      </c>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="108">
+        <v>1</v>
+      </c>
+      <c r="U7" s="108">
+        <v>1</v>
+      </c>
+      <c r="V7" s="109"/>
+      <c r="W7" s="109"/>
+      <c r="X7" s="109"/>
+      <c r="Y7" s="108">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="108">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="108">
+        <v>5000</v>
+      </c>
+      <c r="AB7" s="108">
+        <v>98</v>
+      </c>
+      <c r="AC7" s="108">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="108" t="s">
+        <v>258</v>
+      </c>
+      <c r="AE7" s="108"/>
+      <c r="AF7" s="108"/>
+      <c r="AG7" s="108"/>
+      <c r="AH7" s="108"/>
+    </row>
+    <row r="8" spans="1:34" ht="15">
+      <c r="A8" s="112">
+        <v>583228</v>
+      </c>
+      <c r="B8" s="113" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="106">
+        <v>727</v>
+      </c>
+      <c r="E8" s="106">
+        <v>369</v>
+      </c>
+      <c r="F8" s="106">
+        <v>320</v>
+      </c>
+      <c r="G8" s="106">
+        <v>2</v>
+      </c>
+      <c r="H8" s="106">
+        <v>10000</v>
+      </c>
+      <c r="I8" s="107" t="s">
+        <v>281</v>
+      </c>
+      <c r="J8" s="106">
+        <v>160</v>
+      </c>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="108"/>
+      <c r="O8" s="108"/>
+      <c r="P8" s="108"/>
+      <c r="Q8" s="108"/>
+      <c r="R8" s="108"/>
+      <c r="S8" s="108"/>
+      <c r="T8" s="108">
+        <v>1</v>
+      </c>
+      <c r="U8" s="108">
+        <v>1</v>
+      </c>
+      <c r="V8" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="W8" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="X8" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y8" s="108"/>
+      <c r="Z8" s="108"/>
+      <c r="AA8" s="108"/>
+      <c r="AB8" s="108"/>
+      <c r="AC8" s="108"/>
+      <c r="AD8" s="108"/>
+      <c r="AE8" s="108"/>
+      <c r="AF8" s="108"/>
+      <c r="AG8" s="108"/>
+      <c r="AH8" s="108"/>
+    </row>
+    <row r="9" spans="1:34" ht="15">
+      <c r="A9" s="114">
+        <v>636898</v>
+      </c>
+      <c r="B9" s="115" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="106">
+        <v>727</v>
+      </c>
+      <c r="E9" s="106">
+        <v>369</v>
+      </c>
+      <c r="F9" s="106">
+        <v>320</v>
+      </c>
+      <c r="G9" s="106">
+        <v>2</v>
+      </c>
+      <c r="H9" s="106">
+        <v>10000</v>
+      </c>
+      <c r="I9" s="107" t="s">
+        <v>281</v>
+      </c>
+      <c r="J9" s="106">
+        <v>160</v>
+      </c>
+      <c r="K9" s="108"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="108"/>
+      <c r="P9" s="108"/>
+      <c r="Q9" s="108"/>
+      <c r="R9" s="108"/>
+      <c r="S9" s="108"/>
+      <c r="T9" s="108">
+        <v>1</v>
+      </c>
+      <c r="U9" s="108">
+        <v>1</v>
+      </c>
+      <c r="V9" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="W9" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="X9" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y9" s="108"/>
+      <c r="Z9" s="108"/>
+      <c r="AA9" s="108"/>
+      <c r="AB9" s="108"/>
+      <c r="AC9" s="108"/>
+      <c r="AD9" s="108"/>
+      <c r="AE9" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF9" s="108">
+        <v>1390</v>
+      </c>
+      <c r="AG9" s="108">
+        <v>10000</v>
+      </c>
+      <c r="AH9" s="108">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78739999999999999" right="0.78739999999999999" top="1.0830692913385827" bottom="1.0830692913385827" header="0.88582519685039363" footer="0.88582519685039363"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AG14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="16" width="15.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" customWidth="1"/>
+    <col min="22" max="22" width="17.5703125" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" customWidth="1"/>
+    <col min="24" max="26" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="45">
+      <c r="A1" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="S1" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="U1" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="W1" s="40" t="s">
+        <v>323</v>
+      </c>
+      <c r="X1" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB1" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC1" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD1" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE1" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF1" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG1" s="39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" s="35">
+        <v>870478</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37">
+        <v>727</v>
+      </c>
+      <c r="K2" s="37">
+        <v>369</v>
+      </c>
+      <c r="L2" s="37">
+        <v>320</v>
+      </c>
+      <c r="M2" s="37">
+        <v>2</v>
+      </c>
+      <c r="N2" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O2" s="52" t="s">
+        <v>325</v>
+      </c>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="37">
+        <v>1</v>
+      </c>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="38">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="41"/>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" s="35">
+        <v>1038991</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37">
+        <v>727</v>
+      </c>
+      <c r="K3" s="37">
+        <v>369</v>
+      </c>
+      <c r="L3" s="37">
+        <v>320</v>
+      </c>
+      <c r="M3" s="37">
+        <v>2</v>
+      </c>
+      <c r="N3" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O3" s="52" t="s">
+        <v>325</v>
+      </c>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41">
+        <v>1000</v>
+      </c>
+      <c r="S3" s="41">
+        <v>1000</v>
+      </c>
+      <c r="T3" s="41"/>
+      <c r="U3" s="37">
+        <v>1</v>
+      </c>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37">
+        <v>1000</v>
+      </c>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
+      <c r="AG3" s="41"/>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" s="35">
+        <v>665893</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36">
+        <v>3561</v>
+      </c>
+      <c r="I4" s="120">
+        <v>44200</v>
+      </c>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
+      <c r="AG4" s="41"/>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" s="35">
+        <v>592970</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" s="37">
+        <v>369</v>
+      </c>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37">
+        <v>727</v>
+      </c>
+      <c r="K5" s="37">
+        <v>369</v>
+      </c>
+      <c r="L5" s="37">
+        <v>320</v>
+      </c>
+      <c r="M5" s="37">
+        <v>2</v>
+      </c>
+      <c r="N5" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O5" s="52" t="s">
+        <v>329</v>
+      </c>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="37">
+        <v>1</v>
+      </c>
+      <c r="V5" s="52" t="s">
+        <v>329</v>
+      </c>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="38"/>
+      <c r="AA5" s="38"/>
+      <c r="AB5" s="38"/>
+      <c r="AC5" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="38">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF5" s="36"/>
+      <c r="AG5" s="41"/>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" s="35">
+        <v>592279</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="C6" s="37">
+        <v>369</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37">
+        <v>727</v>
+      </c>
+      <c r="K6" s="37">
+        <v>369</v>
+      </c>
+      <c r="L6" s="37">
+        <v>320</v>
+      </c>
+      <c r="M6" s="37">
+        <v>2</v>
+      </c>
+      <c r="N6" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O6" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="37">
+        <v>1</v>
+      </c>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
+      <c r="X6" s="37"/>
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="38"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="38">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF6" s="36"/>
+      <c r="AG6" s="41"/>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37">
+        <v>727</v>
+      </c>
+      <c r="K7" s="37">
+        <v>369</v>
+      </c>
+      <c r="L7" s="37">
+        <v>320</v>
+      </c>
+      <c r="M7" s="37">
+        <v>2</v>
+      </c>
+      <c r="N7" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O7" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37">
+        <v>2</v>
+      </c>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37">
+        <v>2</v>
+      </c>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37">
+        <v>1</v>
+      </c>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
+      <c r="AE7" s="41"/>
+      <c r="AF7" s="41"/>
+      <c r="AG7" s="41"/>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
+      <c r="AC8" s="41"/>
+      <c r="AD8" s="41"/>
+      <c r="AE8" s="41"/>
+      <c r="AF8" s="41"/>
+      <c r="AG8" s="37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="41">
+        <v>3679</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
+      <c r="AC9" s="41"/>
+      <c r="AD9" s="41"/>
+      <c r="AE9" s="41"/>
+      <c r="AF9" s="41"/>
+      <c r="AG9" s="41"/>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" s="42"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="37">
+        <v>369</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37">
+        <v>727</v>
+      </c>
+      <c r="K10" s="37">
+        <v>369</v>
+      </c>
+      <c r="L10" s="37">
+        <v>320</v>
+      </c>
+      <c r="M10" s="37">
+        <v>2</v>
+      </c>
+      <c r="N10" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O10" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="37">
+        <v>1</v>
+      </c>
+      <c r="V10" s="37"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="38">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF10" s="41"/>
+      <c r="AG10" s="41"/>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" s="42"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="38">
+        <v>1349</v>
+      </c>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41">
+        <v>2</v>
+      </c>
+      <c r="N11" s="41">
+        <v>500</v>
+      </c>
+      <c r="O11" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="38">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF11" s="41"/>
+      <c r="AG11" s="41"/>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="37">
+        <v>369</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37">
+        <v>727</v>
+      </c>
+      <c r="K12" s="37">
+        <v>369</v>
+      </c>
+      <c r="L12" s="37">
+        <v>320</v>
+      </c>
+      <c r="M12" s="37">
+        <v>2</v>
+      </c>
+      <c r="N12" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O12" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="37">
+        <v>1</v>
+      </c>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+      <c r="Z12" s="41"/>
+      <c r="AA12" s="41">
+        <v>3455</v>
+      </c>
+      <c r="AB12" s="41">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="38">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF12" s="41"/>
+      <c r="AG12" s="41"/>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37">
+        <v>727</v>
+      </c>
+      <c r="K13" s="37">
+        <v>369</v>
+      </c>
+      <c r="L13" s="37">
+        <v>320</v>
+      </c>
+      <c r="M13" s="37">
+        <v>2</v>
+      </c>
+      <c r="N13" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O13" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="41"/>
+      <c r="AB13" s="41"/>
+      <c r="AC13" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="38">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF13" s="41"/>
+      <c r="AG13" s="41"/>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37">
+        <v>727</v>
+      </c>
+      <c r="K14" s="37">
+        <v>369</v>
+      </c>
+      <c r="L14" s="37">
+        <v>320</v>
+      </c>
+      <c r="M14" s="37">
+        <v>2</v>
+      </c>
+      <c r="N14" s="37">
+        <v>10000</v>
+      </c>
+      <c r="O14" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="37">
+        <v>1</v>
+      </c>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
+      <c r="AC14" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="38">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF14" s="41"/>
+      <c r="AG14" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="13" max="13" style="54" width="13.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="27.109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="16.44140625" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="38.5546875" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="8.88671875" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="27" max="28" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="31" max="31" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13" style="54" collapsed="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="38.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="27" max="28" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="17.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="14.4">
+    <row r="1" spans="1:34" ht="15">
       <c r="A1" s="39" t="s">
         <v>34</v>
       </c>
@@ -5247,7 +7679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -5255,22 +7687,22 @@
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="20.88671875" collapsed="true"/>
-    <col min="6" max="10" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="23.6640625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="10" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.4">
+    <row r="1" spans="1:20" ht="30">
       <c r="A1" s="39" t="s">
         <v>34</v>
       </c>
@@ -5549,7 +7981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K300"/>
   <sheetViews>
@@ -5557,21 +7989,21 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4">
+    <row r="1" spans="1:11" ht="15">
       <c r="A1" s="39" t="s">
         <v>34</v>
       </c>
@@ -6617,7 +9049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P8"/>
   <sheetViews>
@@ -6625,17 +9057,17 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.4">
+    <row r="1" spans="1:16" ht="15">
       <c r="A1" s="39" t="s">
         <v>34</v>
       </c>
@@ -6809,7 +9241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK27"/>
   <sheetViews>
@@ -6817,34 +9249,34 @@
       <selection activeCell="L3" sqref="L3:Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.88671875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.44140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="14" max="15" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.44140625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="19.77734375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="22.77734375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="20.33203125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="23.77734375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="19.77734375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="96" width="17.88671875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="15" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="17.85546875" style="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="14.4">
+    <row r="1" spans="1:37" ht="15">
       <c r="A1" s="39" t="s">
         <v>34</v>
       </c>
@@ -7395,7 +9827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH11"/>
   <sheetViews>
@@ -7403,28 +9835,27 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="96" width="13.44140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.23828125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.42578125" style="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="14.4">
+    <row r="1" spans="1:34" ht="15">
       <c r="A1" s="39" t="s">
         <v>34</v>
       </c>
@@ -7615,7 +10046,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="78" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P4" s="78"/>
       <c r="Q4" s="36" t="s">
@@ -7800,156 +10231,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="10" max="12" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="11.44140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" ht="14.4">
-      <c r="A1" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="L1" s="40" t="s">
-        <v>256</v>
-      </c>
-      <c r="M1" s="40" t="s">
-        <v>257</v>
-      </c>
-      <c r="N1" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" s="40" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q1" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="R1" s="40" t="s">
-        <v>216</v>
-      </c>
-      <c r="S1" s="40" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="46" t="s">
-        <v>253</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>254</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="37">
-        <v>727</v>
-      </c>
-      <c r="E2" s="37">
-        <v>369</v>
-      </c>
-      <c r="F2" s="37">
-        <v>320</v>
-      </c>
-      <c r="G2" s="37">
-        <v>2</v>
-      </c>
-      <c r="H2" s="37">
-        <v>10000</v>
-      </c>
-      <c r="I2" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="J2" s="87">
-        <v>2</v>
-      </c>
-      <c r="K2" s="87">
-        <v>98</v>
-      </c>
-      <c r="L2" s="87">
-        <v>2</v>
-      </c>
-      <c r="M2" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="N2" s="37">
-        <v>1</v>
-      </c>
-      <c r="O2" s="37">
-        <v>1</v>
-      </c>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="R2" s="36" t="s">
-        <v>218</v>
-      </c>
-      <c r="S2" s="36" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
@@ -7958,12 +10239,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="137.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="137.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="33.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="42.88671875" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="137.6640625" collapsed="true"/>
+    <col min="1" max="1" width="21" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="137.7109375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7977,7 +10258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8">
+    <row r="2" spans="1:3" ht="30">
       <c r="A2" s="5"/>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -7986,7 +10267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8">
+    <row r="3" spans="1:3" ht="30">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -7995,7 +10276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8">
+    <row r="4" spans="1:3" ht="30">
       <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -8004,7 +10285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
@@ -8016,6 +10297,156 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="7.5381999999999998" bottom="7.5381999999999998" header="7.3412999999999995" footer="7.3412999999999995"/>
   <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15">
+      <c r="A1" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="M1" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="N1" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="40" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="S1" s="40" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="46" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="37">
+        <v>727</v>
+      </c>
+      <c r="E2" s="37">
+        <v>369</v>
+      </c>
+      <c r="F2" s="37">
+        <v>320</v>
+      </c>
+      <c r="G2" s="37">
+        <v>2</v>
+      </c>
+      <c r="H2" s="37">
+        <v>10000</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="87">
+        <v>2</v>
+      </c>
+      <c r="K2" s="87">
+        <v>98</v>
+      </c>
+      <c r="L2" s="87">
+        <v>2</v>
+      </c>
+      <c r="M2" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="N2" s="37">
+        <v>1</v>
+      </c>
+      <c r="O2" s="37">
+        <v>1</v>
+      </c>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="R2" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="S2" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8027,16 +10458,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.4">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
@@ -8053,7 +10484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
@@ -8070,7 +10501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="11" t="s">
         <v>20</v>
       </c>
@@ -8105,14 +10536,14 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="3" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.4">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
@@ -8129,7 +10560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="11" t="s">
         <v>22</v>
       </c>
@@ -8146,7 +10577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
@@ -8175,150 +10606,490 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="11.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" style="13" width="10.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="13" width="15.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="13" width="12.6640625" collapsed="true"/>
-    <col min="6" max="16384" style="13" width="10.44140625" collapsed="true"/>
+    <col min="1" max="1" width="13.42578125" style="117" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="117" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="117" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="117" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="117" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.28515625" style="117"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="116" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12">
+      <c r="B2" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="118">
+        <v>123</v>
+      </c>
+      <c r="D2" s="118">
+        <v>1</v>
+      </c>
+      <c r="E2" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="118" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="118" t="s">
+        <v>289</v>
+      </c>
+      <c r="C3" s="118">
         <v>321</v>
       </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="D3" s="118">
+        <v>1</v>
+      </c>
+      <c r="E3" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="118" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" s="118" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="118">
+        <v>321</v>
+      </c>
+      <c r="D4" s="118">
+        <v>1</v>
+      </c>
+      <c r="E4" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="118" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C5" s="118">
         <v>321</v>
       </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="D5" s="118">
+        <v>1</v>
+      </c>
+      <c r="E5" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="118" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6" s="118" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" s="118">
+        <v>321</v>
+      </c>
+      <c r="D6" s="118">
+        <v>1</v>
+      </c>
+      <c r="E6" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="118" t="s">
+        <v>295</v>
+      </c>
+      <c r="B7" s="118" t="s">
+        <v>296</v>
+      </c>
+      <c r="C7" s="118">
+        <v>321</v>
+      </c>
+      <c r="D7" s="118">
+        <v>1</v>
+      </c>
+      <c r="E7" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="118" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" s="118" t="s">
+        <v>298</v>
+      </c>
+      <c r="C8" s="118">
+        <v>321</v>
+      </c>
+      <c r="D8" s="118">
+        <v>1</v>
+      </c>
+      <c r="E8" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="118" t="s">
+        <v>299</v>
+      </c>
+      <c r="B9" s="118" t="s">
+        <v>300</v>
+      </c>
+      <c r="C9" s="118">
+        <v>321</v>
+      </c>
+      <c r="D9" s="118">
+        <v>1</v>
+      </c>
+      <c r="E9" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="118" t="s">
+        <v>301</v>
+      </c>
+      <c r="B10" s="118" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" s="118">
+        <v>321</v>
+      </c>
+      <c r="D10" s="118">
+        <v>1</v>
+      </c>
+      <c r="E10" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="118" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" s="118" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" s="118">
+        <v>321</v>
+      </c>
+      <c r="D11" s="118">
+        <v>1</v>
+      </c>
+      <c r="E11" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="118" t="s">
+        <v>305</v>
+      </c>
+      <c r="B12" s="118" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" s="118">
+        <v>321</v>
+      </c>
+      <c r="D12" s="118">
+        <v>1</v>
+      </c>
+      <c r="E12" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="118" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" s="118">
+        <v>321</v>
+      </c>
+      <c r="D13" s="118">
+        <v>1</v>
+      </c>
+      <c r="E13" s="118">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="1.6355" bottom="1.6355" header="1.4386000000000001" footer="1.4386000000000001"/>
+  <pageMargins left="0.7" right="0.7" top="1.045275590551181" bottom="1.045275590551181" header="0.84842519685039375" footer="0.84842519685039375"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="18.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" style="13" width="10.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="13" width="15.44140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="13" width="12.6640625" collapsed="true"/>
-    <col min="6" max="16384" style="13" width="10.44140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="117" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="117" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="117" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="117" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="117" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.28515625" style="117"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="119" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="118" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="118">
         <v>123</v>
       </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12">
+      <c r="D2" s="118">
+        <v>1</v>
+      </c>
+      <c r="E2" s="118">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="118" t="s">
+        <v>289</v>
+      </c>
+      <c r="C3" s="118">
+        <v>321</v>
+      </c>
+      <c r="D3" s="118">
+        <v>1</v>
+      </c>
+      <c r="E3" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="118" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" s="118" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="118">
+        <v>321</v>
+      </c>
+      <c r="D4" s="118">
+        <v>1</v>
+      </c>
+      <c r="E4" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="118" t="s">
+        <v>310</v>
+      </c>
+      <c r="B5" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C5" s="118">
         <v>321</v>
       </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
+      <c r="D5" s="118">
+        <v>1</v>
+      </c>
+      <c r="E5" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="118" t="s">
+        <v>311</v>
+      </c>
+      <c r="B6" s="118" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" s="118">
+        <v>321</v>
+      </c>
+      <c r="D6" s="118">
+        <v>1</v>
+      </c>
+      <c r="E6" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="118" t="s">
+        <v>312</v>
+      </c>
+      <c r="B7" s="118" t="s">
+        <v>296</v>
+      </c>
+      <c r="C7" s="118">
+        <v>321</v>
+      </c>
+      <c r="D7" s="118">
+        <v>1</v>
+      </c>
+      <c r="E7" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="118" t="s">
+        <v>313</v>
+      </c>
+      <c r="B8" s="118" t="s">
+        <v>298</v>
+      </c>
+      <c r="C8" s="118">
+        <v>321</v>
+      </c>
+      <c r="D8" s="118">
+        <v>1</v>
+      </c>
+      <c r="E8" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="118" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" s="118" t="s">
+        <v>300</v>
+      </c>
+      <c r="C9" s="118">
+        <v>321</v>
+      </c>
+      <c r="D9" s="118">
+        <v>1</v>
+      </c>
+      <c r="E9" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="118" t="s">
+        <v>315</v>
+      </c>
+      <c r="B10" s="118" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" s="118">
+        <v>321</v>
+      </c>
+      <c r="D10" s="118">
+        <v>1</v>
+      </c>
+      <c r="E10" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="118" t="s">
+        <v>316</v>
+      </c>
+      <c r="B11" s="118" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" s="118">
+        <v>321</v>
+      </c>
+      <c r="D11" s="118">
+        <v>1</v>
+      </c>
+      <c r="E11" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="118" t="s">
+        <v>317</v>
+      </c>
+      <c r="B12" s="118" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" s="118">
+        <v>321</v>
+      </c>
+      <c r="D12" s="118">
+        <v>1</v>
+      </c>
+      <c r="E12" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="118" t="s">
+        <v>318</v>
+      </c>
+      <c r="B13" s="118" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" s="118">
+        <v>321</v>
+      </c>
+      <c r="D13" s="118">
+        <v>1</v>
+      </c>
+      <c r="E13" s="118">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="1.6355" bottom="1.6355" header="1.4386000000000001" footer="1.4386000000000001"/>
+  <pageMargins left="0.7" right="0.7" top="1.045275590551181" bottom="1.045275590551181" header="0.84842519685039375" footer="0.84842519685039375"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
@@ -8331,13 +11102,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.33203125" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.109375" collapsed="true"/>
-    <col min="2" max="5" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="1" max="1" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.4">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="14" t="s">
         <v>13</v>
       </c>
@@ -8354,7 +11125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
@@ -8371,7 +11142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="12" t="s">
         <v>28</v>
       </c>
@@ -8406,11 +11177,11 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="12.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="13" width="11.33203125" collapsed="true"/>
-    <col min="3" max="16384" style="13" width="10.44140625" collapsed="true"/>
+    <col min="1" max="1" width="12.7109375" style="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="10.42578125" style="13" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8460,17 +11231,17 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="44.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="44.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="23" width="10.6640625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="23" width="15.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="23" width="16.109375" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" style="23" width="29.88671875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="23" width="31.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="23" width="30.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="23" width="29.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="23" width="28.88671875" collapsed="true"/>
-    <col min="11" max="16384" style="23" width="44.6640625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" style="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.28515625" style="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" style="23" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.85546875" style="23" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.5703125" style="23" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.28515625" style="23" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29.85546875" style="23" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="28.85546875" style="23" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="44.7109375" style="23" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" customHeight="1">

</xml_diff>